<commit_message>
Funcionando bien en MAMP/WAMP. Pero sólo con versiones antiguas de PHP y con un CSS original
</commit_message>
<xml_diff>
--- a/cursos/2021-2022/alumnos/1_SEA-CIE.xlsx
+++ b/cursos/2021-2022/alumnos/1_SEA-CIE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10315"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cferrerobonet/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cferrerobonet/Documents/04 DESARROLLADOR/Web/EPLA/AUTOEXAM/cursos/2021-2022/alumnos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1095AB34-69ED-7045-9A96-0912D2722941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C94E399-623F-214B-96AC-CF02B600E1DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13440" yWindow="760" windowWidth="16800" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>ASIGNATURA:</t>
   </si>
@@ -42,76 +42,7 @@
     <t>ALUMNOS:</t>
   </si>
   <si>
-    <t>ADÁN GATELL, BRIAN ELÍAS</t>
-  </si>
-  <si>
-    <t>ANDOMBE OBAMA, LAUREN</t>
-  </si>
-  <si>
-    <t>ARAIXA HERNÁNDEZ, RAÚL</t>
-  </si>
-  <si>
-    <t>BONORA VALERO, FRANCISCO</t>
-  </si>
-  <si>
-    <t>COLLADO ROSSI, ALEJANDRO</t>
-  </si>
-  <si>
-    <t>GARAÑANA DOMÉNECH, CRISTIAN</t>
-  </si>
-  <si>
-    <t>HERRERA SERRANO, LAURA</t>
-  </si>
-  <si>
-    <t>ISIDRO AVILÉS, ÁLVARO</t>
-  </si>
-  <si>
-    <t>KOUTAIBI , OMAR</t>
-  </si>
-  <si>
-    <t>MARCO ARAQUE, JOSÉ IGNACIO</t>
-  </si>
-  <si>
-    <t>MARGAIX ALCOVER, XIMO</t>
-  </si>
-  <si>
-    <t>MARTÍNEZ BACA, FRANCISCO JUAN</t>
-  </si>
-  <si>
-    <t>MARTÍNEZ MUÑOZ, CARLOS</t>
-  </si>
-  <si>
-    <t>MORÓN JUANES, JOSÉ VICENTE</t>
-  </si>
-  <si>
-    <t>PEÑA AMBLAR, JOAN</t>
-  </si>
-  <si>
-    <t>RAMÍREZ HEREDIA, EDWARD ISMAEL</t>
-  </si>
-  <si>
-    <t>REQUENI MARTÍNEZ, ALEJANDRO</t>
-  </si>
-  <si>
-    <t>RODRÍGUEZ BASSO, STEVEN MAXIMILIANO</t>
-  </si>
-  <si>
-    <t>SEPÚLVEDA ANDRÉS, RAMÓN MANUEL</t>
-  </si>
-  <si>
-    <t>TAMARIT JÁVEGA, DAVID</t>
-  </si>
-  <si>
-    <t>TOLEDO ÁLVAREZ, ANA</t>
-  </si>
-  <si>
-    <t>TORRES MARTÍNEZ, CARLOS</t>
-  </si>
-  <si>
     <t>_Ferrero Bonet, Carlos</t>
-  </si>
-  <si>
-    <t>BELLMUNT GALVIS, jAVIER</t>
   </si>
 </sst>
 </file>
@@ -170,17 +101,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:XFC27"/>
+  <dimension ref="A1:XFC4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -482,8 +407,8 @@
       </c>
     </row>
     <row r="2" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="3"/>
       <c r="C2" s="1"/>
       <c r="E2" s="1"/>
       <c r="G2" s="1"/>
@@ -8682,143 +8607,8 @@
       </c>
     </row>
     <row r="4" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="A4" t="s">
         <v>3</v>
-      </c>
-      <c r="B4" s="2"/>
-    </row>
-    <row r="5" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2"/>
-    </row>
-    <row r="7" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="2"/>
-    </row>
-    <row r="8" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="2"/>
-    </row>
-    <row r="11" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="2"/>
-    </row>
-    <row r="12" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="2"/>
-    </row>
-    <row r="13" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="2"/>
-    </row>
-    <row r="14" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="2"/>
-    </row>
-    <row r="15" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="2"/>
-    </row>
-    <row r="16" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="2"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="2"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="2"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="2"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="2"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="2"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="2"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="2"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>